<commit_message>
added second version of requirements
</commit_message>
<xml_diff>
--- a/ontology/requirements/requirements.xlsx
+++ b/ontology/requirements/requirements.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\rml-lv\ontology\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AC0C4C-B250-4D83-8B91-5459A7536ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40558EE-7E8E-401B-B117-0231488D52D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="version 1" sheetId="1" r:id="rId1"/>
+    <sheet name="version 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Identifier</t>
   </si>
@@ -77,9 +78,6 @@
     <t>rml-lv-r6</t>
   </si>
   <si>
-    <t>Create references to the position of a data record in a logical iteration</t>
-  </si>
-  <si>
     <t>Describe structural properties of data records</t>
   </si>
   <si>
@@ -90,6 +88,45 @@
   </si>
   <si>
     <t xml:space="preserve">rml-lv &amp; mapping challenge C5b </t>
+  </si>
+  <si>
+    <t>rml-lv-r7</t>
+  </si>
+  <si>
+    <t>Create a reference to the position of a data record in a sequence of data records</t>
+  </si>
+  <si>
+    <t>A logical view describes a source format agnostic view over a data soure</t>
+  </si>
+  <si>
+    <t>A field gives a name to data records derived from a data source</t>
+  </si>
+  <si>
+    <t>A nested field may flatten a nested data source</t>
+  </si>
+  <si>
+    <t>An iterable field may define a new reference formulation and iterator</t>
+  </si>
+  <si>
+    <t>A logical view join may add fields from another logical view to a logical view subjected to zero or more join conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An expression may reference a field name of an  expression field to retrieve the value of the data records defined by that field. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An expression  may the index of a field or abstract logical source of a logical view may to retrieve the position of a data record or logical iteration with a sequence of data records or logical iterations. </t>
+  </si>
+  <si>
+    <t>rml-lv-r8</t>
+  </si>
+  <si>
+    <t>rml-lv-r9</t>
+  </si>
+  <si>
+    <t>A field may describe structural properties of data records</t>
+  </si>
+  <si>
+    <t>A field may describe structural relations between data records</t>
   </si>
 </sst>
 </file>
@@ -472,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD387039-14E8-1C40-88EB-6D939C392012}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -501,7 +538,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -512,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -526,12 +563,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -542,7 +579,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -553,7 +590,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -588,6 +625,169 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1641CC76-0306-4500-8F84-3516D2E66764}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="60.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
splitting requirements.xlsx in 2 versions
</commit_message>
<xml_diff>
--- a/ontology/requirements/requirements.xlsx
+++ b/ontology/requirements/requirements.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\rml-lv\ontology\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40558EE-7E8E-401B-B117-0231488D52D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485E2CB-77A7-43DE-BA1E-B75DDAAB413C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="version 1" sheetId="1" r:id="rId1"/>
-    <sheet name="version 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Identifier</t>
   </si>
@@ -60,15 +59,6 @@
     <t>rml-lv</t>
   </si>
   <si>
-    <t>Flatten a nested data source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Join two or more data sources </t>
-  </si>
-  <si>
-    <t>Handle data sources with mixed data formats</t>
-  </si>
-  <si>
     <t>rml-lv-r4</t>
   </si>
   <si>
@@ -78,12 +68,6 @@
     <t>rml-lv-r6</t>
   </si>
   <si>
-    <t>Describe structural properties of data records</t>
-  </si>
-  <si>
-    <t>Describe structural relations between data records</t>
-  </si>
-  <si>
     <t>rml-lv &amp; mapping challenge C2a</t>
   </si>
   <si>
@@ -91,9 +75,6 @@
   </si>
   <si>
     <t>rml-lv-r7</t>
-  </si>
-  <si>
-    <t>Create a reference to the position of a data record in a sequence of data records</t>
   </si>
   <si>
     <t>A logical view describes a source format agnostic view over a data soure</t>
@@ -506,11 +487,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD387039-14E8-1C40-88EB-6D939C392012}">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1641CC76-0306-4500-8F84-3516D2E66764}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -530,15 +511,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -546,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -557,178 +538,51 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1641CC76-0306-4500-8F84-3516D2E66764}">
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="60.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="8" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -736,10 +590,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -747,10 +601,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Preparation of publication (#55)
## What's changed
<!-- Give a concise description of the change -->
prepares spec for publication
splits requirements.xlsx into 2 versions 

## Change checklist
- [x] updated ontology, where necessary
- [x] updated shapes, where necessary
- [x] added or updated test cases, where necessary
- [x] any TODOs have been turned into trackable issues and referenced
where necessary

## Issue reference
<!-- For example: -->
<!-- Fixes #{ISSUE}. -->
<!-- Resolves #{ISSUE}. -->
</commit_message>
<xml_diff>
--- a/ontology/requirements/requirements.xlsx
+++ b/ontology/requirements/requirements.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\rml-lv\ontology\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40558EE-7E8E-401B-B117-0231488D52D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485E2CB-77A7-43DE-BA1E-B75DDAAB413C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="version 1" sheetId="1" r:id="rId1"/>
-    <sheet name="version 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Identifier</t>
   </si>
@@ -60,15 +59,6 @@
     <t>rml-lv</t>
   </si>
   <si>
-    <t>Flatten a nested data source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Join two or more data sources </t>
-  </si>
-  <si>
-    <t>Handle data sources with mixed data formats</t>
-  </si>
-  <si>
     <t>rml-lv-r4</t>
   </si>
   <si>
@@ -78,12 +68,6 @@
     <t>rml-lv-r6</t>
   </si>
   <si>
-    <t>Describe structural properties of data records</t>
-  </si>
-  <si>
-    <t>Describe structural relations between data records</t>
-  </si>
-  <si>
     <t>rml-lv &amp; mapping challenge C2a</t>
   </si>
   <si>
@@ -91,9 +75,6 @@
   </si>
   <si>
     <t>rml-lv-r7</t>
-  </si>
-  <si>
-    <t>Create a reference to the position of a data record in a sequence of data records</t>
   </si>
   <si>
     <t>A logical view describes a source format agnostic view over a data soure</t>
@@ -506,11 +487,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD387039-14E8-1C40-88EB-6D939C392012}">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1641CC76-0306-4500-8F84-3516D2E66764}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -530,15 +511,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -546,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -557,178 +538,51 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1641CC76-0306-4500-8F84-3516D2E66764}">
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="60.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="8" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -736,10 +590,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -747,10 +601,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>

</xml_diff>